<commit_message>
some fixes and japan civvies
</commit_message>
<xml_diff>
--- a/Modding resources/mineral calculations/size_modifier.xlsx
+++ b/Modding resources/mineral calculations/size_modifier.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Revised</t>
-  </si>
-  <si>
     <t>Civ IC 2017</t>
   </si>
   <si>
@@ -79,39 +76,15 @@
     <t>India</t>
   </si>
   <si>
-    <t>ger</t>
-  </si>
-  <si>
-    <t>uk</t>
-  </si>
-  <si>
-    <t>rus</t>
-  </si>
-  <si>
     <t>ino</t>
   </si>
   <si>
-    <t>ita</t>
-  </si>
-  <si>
-    <t>spa</t>
-  </si>
-  <si>
     <t>Poland</t>
   </si>
   <si>
-    <t>hol</t>
-  </si>
-  <si>
     <t>Iran</t>
   </si>
   <si>
-    <t>phi</t>
-  </si>
-  <si>
-    <t>sau</t>
-  </si>
-  <si>
     <t>saf</t>
   </si>
   <si>
@@ -251,6 +224,24 @@
   </si>
   <si>
     <t>Then remove mil IC from all useless nations once system is done</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Philipinnes</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
   </si>
 </sst>
 </file>
@@ -658,7 +649,7 @@
   <dimension ref="A1:T213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="14.25"/>
@@ -679,28 +670,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
       </c>
       <c r="J2">
         <v>0.01</v>
@@ -709,27 +700,30 @@
         <v>0.25</v>
       </c>
       <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" t="s">
+      <c r="R2" t="s">
         <v>11</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>12</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>13</v>
-      </c>
-      <c r="T2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
       </c>
       <c r="C3">
         <v>210</v>
@@ -768,7 +762,7 @@
         <v>59.158904109589002</v>
       </c>
       <c r="O3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P3">
         <v>0</v>
@@ -788,13 +782,13 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
         <v>175</v>
-      </c>
-      <c r="C4">
-        <v>144</v>
       </c>
       <c r="D4">
         <v>27.789866074966302</v>
@@ -830,7 +824,7 @@
         <v>69.145205479452102</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="P4">
         <v>1</v>
@@ -850,7 +844,7 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5">
         <v>72</v>
@@ -906,7 +900,7 @@
     </row>
     <row r="6" spans="1:20">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>66</v>
@@ -962,7 +956,7 @@
     </row>
     <row r="7" spans="1:20">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>56</v>
@@ -1018,7 +1012,7 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C8">
         <v>40</v>
@@ -1074,7 +1068,7 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="C9">
         <v>39</v>
@@ -1130,7 +1124,7 @@
     </row>
     <row r="10" spans="1:20">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>35</v>
@@ -1186,7 +1180,7 @@
     </row>
     <row r="11" spans="1:20">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="C11">
         <v>30</v>
@@ -1242,7 +1236,7 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="C12">
         <v>25</v>
@@ -1298,7 +1292,7 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C13">
         <v>18</v>
@@ -1354,7 +1348,7 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="C14">
         <v>15</v>
@@ -1410,7 +1404,7 @@
     </row>
     <row r="15" spans="1:20">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -1466,7 +1460,7 @@
     </row>
     <row r="16" spans="1:20">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="C16">
         <v>13</v>
@@ -1522,7 +1516,7 @@
     </row>
     <row r="17" spans="1:20">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -1578,7 +1572,7 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C18">
         <v>11</v>
@@ -1634,7 +1628,7 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C19">
         <v>11</v>
@@ -1690,7 +1684,7 @@
     </row>
     <row r="20" spans="1:20">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C20">
         <v>11</v>
@@ -1746,7 +1740,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C21">
         <v>11</v>
@@ -1802,7 +1796,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C22">
         <v>9</v>
@@ -1858,7 +1852,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>8</v>
@@ -1914,7 +1908,7 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C24">
         <v>8</v>
@@ -1970,7 +1964,7 @@
     </row>
     <row r="25" spans="1:20">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C25">
         <v>7</v>
@@ -2026,7 +2020,7 @@
     </row>
     <row r="26" spans="1:20">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C26">
         <v>7</v>
@@ -2082,7 +2076,7 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -2138,7 +2132,7 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>6</v>
@@ -2194,7 +2188,7 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -2250,7 +2244,7 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C30">
         <v>6</v>
@@ -2306,7 +2300,7 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C31">
         <v>6</v>
@@ -2362,7 +2356,7 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C32">
         <v>6</v>
@@ -2418,7 +2412,7 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -2474,7 +2468,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -2530,7 +2524,7 @@
     </row>
     <row r="35" spans="1:20">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -2586,7 +2580,7 @@
     </row>
     <row r="36" spans="1:20">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>3</v>
@@ -2642,7 +2636,7 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2698,7 +2692,7 @@
     </row>
     <row r="38" spans="1:20">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2754,7 +2748,7 @@
     </row>
     <row r="39" spans="1:20">
       <c r="A39" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2810,7 +2804,7 @@
     </row>
     <row r="40" spans="1:20">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -3070,7 +3064,7 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="P53">
         <v>95</v>
@@ -3405,19 +3399,19 @@
     </row>
     <row r="81" spans="1:20">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C81" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="F81" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="G81" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="I81" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="S81">
         <v>78</v>
@@ -3428,7 +3422,7 @@
     </row>
     <row r="82" spans="1:20">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C82">
         <v>98</v>
@@ -3442,7 +3436,7 @@
     </row>
     <row r="83" spans="1:20">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C83">
         <v>52</v>
@@ -3456,7 +3450,7 @@
     </row>
     <row r="84" spans="1:20">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C84">
         <v>51</v>
@@ -3470,7 +3464,7 @@
     </row>
     <row r="85" spans="1:20">
       <c r="A85" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C85">
         <v>26</v>
@@ -3484,7 +3478,7 @@
     </row>
     <row r="86" spans="1:20">
       <c r="A86" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C86">
         <v>24</v>
@@ -3498,7 +3492,7 @@
     </row>
     <row r="87" spans="1:20">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C87">
         <v>26</v>
@@ -3512,7 +3506,7 @@
     </row>
     <row r="88" spans="1:20">
       <c r="A88" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C88">
         <v>18</v>
@@ -3526,7 +3520,7 @@
     </row>
     <row r="89" spans="1:20">
       <c r="A89" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C89">
         <v>10</v>
@@ -3540,7 +3534,7 @@
     </row>
     <row r="90" spans="1:20">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C90">
         <v>20</v>
@@ -3554,7 +3548,7 @@
     </row>
     <row r="91" spans="1:20">
       <c r="A91" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C91">
         <v>16</v>
@@ -3568,7 +3562,7 @@
     </row>
     <row r="92" spans="1:20">
       <c r="A92" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="C92">
         <v>7</v>
@@ -3582,7 +3576,7 @@
     </row>
     <row r="93" spans="1:20">
       <c r="A93" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C93">
         <v>4</v>
@@ -3596,7 +3590,7 @@
     </row>
     <row r="94" spans="1:20">
       <c r="A94" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C94">
         <v>12</v>
@@ -3610,7 +3604,7 @@
     </row>
     <row r="95" spans="1:20">
       <c r="A95" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C95">
         <v>15</v>
@@ -3624,7 +3618,7 @@
     </row>
     <row r="96" spans="1:20">
       <c r="A96" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C96">
         <v>7</v>
@@ -3638,7 +3632,7 @@
     </row>
     <row r="97" spans="1:20">
       <c r="A97" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C97">
         <v>8</v>
@@ -3652,7 +3646,7 @@
     </row>
     <row r="98" spans="1:20">
       <c r="A98" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C98">
         <v>6</v>
@@ -3666,7 +3660,7 @@
     </row>
     <row r="99" spans="1:20">
       <c r="A99" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="C99">
         <v>9</v>
@@ -3680,7 +3674,7 @@
     </row>
     <row r="100" spans="1:20">
       <c r="A100" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C100">
         <v>9</v>
@@ -3694,7 +3688,7 @@
     </row>
     <row r="101" spans="1:20">
       <c r="A101" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="C101">
         <v>4</v>
@@ -3708,7 +3702,7 @@
     </row>
     <row r="102" spans="1:20">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C102">
         <v>4</v>
@@ -3722,7 +3716,7 @@
     </row>
     <row r="103" spans="1:20">
       <c r="A103" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="S103">
         <v>100</v>

</xml_diff>

<commit_message>
GER and ENG civvies finished
</commit_message>
<xml_diff>
--- a/Modding resources/mineral calculations/size_modifier.xlsx
+++ b/Modding resources/mineral calculations/size_modifier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -649,7 +649,7 @@
   <dimension ref="A1:T213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="14.25"/>
@@ -846,6 +846,9 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
       <c r="C5">
         <v>72</v>
       </c>
@@ -902,6 +905,9 @@
       <c r="A6" t="s">
         <v>19</v>
       </c>
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
       <c r="C6">
         <v>66</v>
       </c>
@@ -958,6 +964,9 @@
       <c r="A7" t="s">
         <v>53</v>
       </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
       <c r="C7">
         <v>56</v>
       </c>
@@ -1013,6 +1022,9 @@
     <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>72</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
       </c>
       <c r="C8">
         <v>40</v>

</xml_diff>

<commit_message>
italy done and some map fixes
</commit_message>
<xml_diff>
--- a/Modding resources/mineral calculations/size_modifier.xlsx
+++ b/Modding resources/mineral calculations/size_modifier.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -649,7 +649,7 @@
   <dimension ref="A1:T213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.75" defaultRowHeight="14.25"/>
@@ -1082,6 +1082,9 @@
       <c r="A9" t="s">
         <v>52</v>
       </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
       <c r="C9">
         <v>39</v>
       </c>
@@ -1193,6 +1196,9 @@
     <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
       </c>
       <c r="C11">
         <v>30</v>

</xml_diff>